<commit_message>
Change AlternateSSID column header with ExternalSSID
</commit_message>
<xml_diff>
--- a/irp-package/IRPStudents.xlsx
+++ b/irp-package/IRPStudents.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27610"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27907"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Espinosa/Development/SmarterBalanced/irp-automation-adapter-sboss/irp-automation-adapter-sboss-application/src/main/resources/irp-package/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Espinosa/Development/SmarterBalanced/irp-package/irp-package/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -83,9 +83,6 @@
     <t>Birthdate</t>
   </si>
   <si>
-    <t>AlternateSSID</t>
-  </si>
-  <si>
     <t>GradeLevelWhenAssessed</t>
   </si>
   <si>
@@ -234,6 +231,9 @@
   </si>
   <si>
     <t>AIRP79990002</t>
+  </si>
+  <si>
+    <t>ExternalSSID</t>
   </si>
 </sst>
 </file>
@@ -772,9 +772,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AE7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -828,73 +826,73 @@
         <v>0</v>
       </c>
       <c r="I1" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="J1" s="7" t="s">
         <v>18</v>
-      </c>
-      <c r="J1" s="7" t="s">
-        <v>19</v>
       </c>
       <c r="K1" s="7" t="s">
         <v>1</v>
       </c>
       <c r="L1" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="M1" s="7" t="s">
         <v>36</v>
-      </c>
-      <c r="M1" s="7" t="s">
-        <v>37</v>
       </c>
       <c r="N1" s="7" t="s">
         <v>2</v>
       </c>
       <c r="O1" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P1" s="7" t="s">
         <v>3</v>
       </c>
       <c r="Q1" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="R1" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="S1" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="T1" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="U1" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="V1" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="R1" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="S1" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="T1" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="U1" s="7" t="s">
+      <c r="W1" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="V1" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="W1" s="7" t="s">
+      <c r="X1" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="X1" s="7" t="s">
+      <c r="Y1" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="Y1" s="7" t="s">
+      <c r="Z1" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="Z1" s="7" t="s">
+      <c r="AA1" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="AA1" s="7" t="s">
+      <c r="AB1" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="AB1" s="7" t="s">
+      <c r="AC1" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="AC1" s="7" t="s">
+      <c r="AD1" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="AD1" s="2" t="s">
+      <c r="AE1" s="7" t="s">
         <v>32</v>
-      </c>
-      <c r="AE1" s="7" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:31" x14ac:dyDescent="0.2">
@@ -908,61 +906,61 @@
         <v>1</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G2" s="5">
         <v>39508</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K2" s="1" t="s">
         <v>5</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="Q2" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="R2" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="S2" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="T2" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="U2" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="V2" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="W2" s="1" t="s">
         <v>6</v>
@@ -971,7 +969,7 @@
         <v>3</v>
       </c>
       <c r="Y2" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="Z2" s="6">
         <v>40393</v>
@@ -993,59 +991,59 @@
         <v>1</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F3" s="1"/>
       <c r="G3" s="5">
         <v>39509</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K3" s="1" t="s">
         <v>5</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="P3" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="Q3" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="R3" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="S3" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="T3" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="U3" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="V3" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="W3" s="1" t="s">
         <v>6</v>
@@ -1054,7 +1052,7 @@
         <v>3</v>
       </c>
       <c r="Y3" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="Z3" s="6">
         <v>40394</v>
@@ -1076,59 +1074,59 @@
         <v>1</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F4" s="1"/>
       <c r="G4" s="5">
         <v>39510</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="K4" s="1" t="s">
         <v>7</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="O4" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="P4" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="Q4" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="R4" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="S4" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="T4" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="U4" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="V4" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="W4" s="1" t="s">
         <v>6</v>
@@ -1137,7 +1135,7 @@
         <v>3</v>
       </c>
       <c r="Y4" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="Z4" s="6">
         <v>40395</v>
@@ -1159,59 +1157,59 @@
         <v>1</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F5" s="1"/>
       <c r="G5" s="5">
         <v>39511</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="J5" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="K5" s="1" t="s">
         <v>7</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="O5" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="P5" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="Q5" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="R5" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="S5" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="T5" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="U5" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="V5" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="W5" s="1" t="s">
         <v>6</v>
@@ -1220,7 +1218,7 @@
         <v>3</v>
       </c>
       <c r="Y5" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="Z5" s="6">
         <v>40396</v>
@@ -1246,61 +1244,61 @@
         <v>1</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G6" s="5">
         <v>39512</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="J6" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="K6" s="1" t="s">
         <v>5</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="N6" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="O6" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="P6" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="Q6" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="R6" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="S6" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="T6" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="U6" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="V6" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="W6" s="1" t="s">
         <v>6</v>
@@ -1309,7 +1307,7 @@
         <v>3</v>
       </c>
       <c r="Y6" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="Z6" s="6">
         <v>40397</v>
@@ -1331,59 +1329,59 @@
         <v>1</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F7" s="1"/>
       <c r="G7" s="5">
         <v>39513</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J7" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="K7" s="1" t="s">
         <v>5</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="M7" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="N7" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="O7" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="P7" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="Q7" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="R7" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="S7" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="T7" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="U7" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="V7" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="W7" s="1" t="s">
         <v>6</v>
@@ -1392,7 +1390,7 @@
         <v>3</v>
       </c>
       <c r="Y7" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="Z7" s="6">
         <v>40398</v>

</xml_diff>

<commit_message>
Change DUALLANGUAGE to DualLanguage
DualLanguage is correct according to spec
</commit_message>
<xml_diff>
--- a/irp-package/IRPStudents.xlsx
+++ b/irp-package/IRPStudents.xlsx
@@ -59,9 +59,6 @@
     <t>2012-06-13</t>
   </si>
   <si>
-    <t>DUALLANGUAGE</t>
-  </si>
-  <si>
     <t>StateAbbreviation</t>
   </si>
   <si>
@@ -234,6 +231,9 @@
   </si>
   <si>
     <t>ExternalSSID</t>
+  </si>
+  <si>
+    <t>DualLanguage</t>
   </si>
 </sst>
 </file>
@@ -802,97 +802,97 @@
   <sheetData>
     <row r="1" spans="1:31" s="8" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="C1" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="D1" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="E1" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="F1" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="G1" s="7" t="s">
         <v>16</v>
-      </c>
-      <c r="G1" s="7" t="s">
-        <v>17</v>
       </c>
       <c r="H1" s="7" t="s">
         <v>0</v>
       </c>
       <c r="I1" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="J1" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K1" s="7" t="s">
         <v>1</v>
       </c>
       <c r="L1" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="M1" s="7" t="s">
         <v>35</v>
-      </c>
-      <c r="M1" s="7" t="s">
-        <v>36</v>
       </c>
       <c r="N1" s="7" t="s">
         <v>2</v>
       </c>
       <c r="O1" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="P1" s="7" t="s">
         <v>3</v>
       </c>
       <c r="Q1" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="R1" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="S1" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="T1" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="U1" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="V1" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="R1" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="S1" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="T1" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="U1" s="7" t="s">
+      <c r="W1" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="V1" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="W1" s="7" t="s">
+      <c r="X1" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="X1" s="7" t="s">
+      <c r="Y1" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="Y1" s="7" t="s">
+      <c r="Z1" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="Z1" s="7" t="s">
+      <c r="AA1" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="AA1" s="7" t="s">
+      <c r="AB1" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="AB1" s="7" t="s">
+      <c r="AC1" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="AC1" s="7" t="s">
+      <c r="AD1" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="AD1" s="2" t="s">
+      <c r="AE1" s="7" t="s">
         <v>31</v>
-      </c>
-      <c r="AE1" s="7" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:31" x14ac:dyDescent="0.2">
@@ -906,61 +906,61 @@
         <v>1</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G2" s="5">
         <v>39508</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="K2" s="1" t="s">
         <v>5</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="Q2" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="R2" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="S2" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="T2" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="U2" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="V2" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="W2" s="1" t="s">
         <v>6</v>
@@ -969,7 +969,7 @@
         <v>3</v>
       </c>
       <c r="Y2" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="Z2" s="6">
         <v>40393</v>
@@ -991,59 +991,59 @@
         <v>1</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F3" s="1"/>
       <c r="G3" s="5">
         <v>39509</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="K3" s="1" t="s">
         <v>5</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="P3" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="Q3" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="R3" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="S3" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="T3" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="U3" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="V3" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="W3" s="1" t="s">
         <v>6</v>
@@ -1052,7 +1052,7 @@
         <v>3</v>
       </c>
       <c r="Y3" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="Z3" s="6">
         <v>40394</v>
@@ -1074,59 +1074,59 @@
         <v>1</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F4" s="1"/>
       <c r="G4" s="5">
         <v>39510</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="K4" s="1" t="s">
         <v>7</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="M4" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="O4" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="P4" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="Q4" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="R4" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="S4" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="T4" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="U4" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="V4" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="W4" s="1" t="s">
         <v>6</v>
@@ -1135,7 +1135,7 @@
         <v>3</v>
       </c>
       <c r="Y4" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="Z4" s="6">
         <v>40395</v>
@@ -1157,59 +1157,59 @@
         <v>1</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F5" s="1"/>
       <c r="G5" s="5">
         <v>39511</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J5" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="K5" s="1" t="s">
         <v>7</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="O5" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="P5" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="Q5" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="R5" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="S5" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="T5" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="U5" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="V5" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="W5" s="1" t="s">
         <v>6</v>
@@ -1218,7 +1218,7 @@
         <v>3</v>
       </c>
       <c r="Y5" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="Z5" s="6">
         <v>40396</v>
@@ -1230,7 +1230,7 @@
         <v>9</v>
       </c>
       <c r="AC5" s="4" t="s">
-        <v>10</v>
+        <v>68</v>
       </c>
     </row>
     <row r="6" spans="1:31" x14ac:dyDescent="0.2">
@@ -1244,61 +1244,61 @@
         <v>1</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G6" s="5">
         <v>39512</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J6" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="K6" s="1" t="s">
         <v>5</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="N6" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="O6" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="P6" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="Q6" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="R6" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="S6" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="T6" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="U6" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="V6" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="W6" s="1" t="s">
         <v>6</v>
@@ -1307,7 +1307,7 @@
         <v>3</v>
       </c>
       <c r="Y6" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="Z6" s="6">
         <v>40397</v>
@@ -1329,59 +1329,59 @@
         <v>1</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F7" s="1"/>
       <c r="G7" s="5">
         <v>39513</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="J7" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="K7" s="1" t="s">
         <v>5</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="M7" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="N7" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="O7" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="P7" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="Q7" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="R7" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="S7" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="T7" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="U7" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="V7" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="W7" s="1" t="s">
         <v>6</v>
@@ -1390,7 +1390,7 @@
         <v>3</v>
       </c>
       <c r="Y7" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="Z7" s="6">
         <v>40398</v>

</xml_diff>